<commit_message>
Update Psychrophiles and Thermophiles.xlsx
</commit_message>
<xml_diff>
--- a/data/Psychrophiles and Thermophiles.xlsx
+++ b/data/Psychrophiles and Thermophiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aed3d806ed7068fe/Documents/GitHub/TARA-thiolases/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="218" documentId="8_{7ACB10E6-3A25-4D72-9F4B-6E9F0C2BB121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57D3CDB4-32AF-456D-B1C2-E48111C4FC70}"/>
+  <xr:revisionPtr revIDLastSave="284" documentId="8_{7ACB10E6-3A25-4D72-9F4B-6E9F0C2BB121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F7D017F3-F6F7-47BB-9E46-B1FA95DC3ACF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6D20BB76-7F3F-49CF-9972-83C8C9A32C4D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="227">
   <si>
     <t>to_synthesize</t>
   </si>
@@ -374,9 +374,6 @@
     <t>Thermophilic</t>
   </si>
   <si>
-    <t>50-55</t>
-  </si>
-  <si>
     <t>Candidatus Riflebacteria bacterium BY5</t>
   </si>
   <si>
@@ -428,9 +425,6 @@
     <t>fig|326427.4.peg.557</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Deltaproteobacteria bacterium strain B30_G6</t>
   </si>
   <si>
@@ -654,13 +648,79 @@
   </si>
   <si>
     <t>"cold room"</t>
+  </si>
+  <si>
+    <t>https://bacdive.dsmz.de/strain/431</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/Taxonomy/Browser/wwwtax.cgi?id=1220571</t>
+  </si>
+  <si>
+    <t>https://www.nite.go.jp/nbrc/catalogue/NBRCCatalogueDetailServlet?ID=NBRC&amp;CAT=00103104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Kakegawa, Shizuoka</t>
+  </si>
+  <si>
+    <t>Soil in a field</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1099/ijs.0.64692-0</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1093/femsec/fiy152</t>
+  </si>
+  <si>
+    <t>Tomsk Region of the Western Siberia, Russia.</t>
+  </si>
+  <si>
+    <t>55 C</t>
+  </si>
+  <si>
+    <t>50-55 C</t>
+  </si>
+  <si>
+    <t>57 C</t>
+  </si>
+  <si>
+    <t>Okukinu Meotobuchi hot spring in Tochigi Prefecture, Japan.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1099/00207713-45-4-676</t>
+  </si>
+  <si>
+    <t>50-60 C</t>
+  </si>
+  <si>
+    <t>all seem to be from the same source but I can't find it</t>
+  </si>
+  <si>
+    <t>patric seems to be pulling data about Mastigocladus laminosus, is that the same thing?</t>
+  </si>
+  <si>
+    <t>DOI: 10.4056/sigs.1533840</t>
+  </si>
+  <si>
+    <t>41 C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Kah-nee-tah Hot Spring, Oregon,USA</t>
+  </si>
+  <si>
+    <t>44.86 N, 121.20 W</t>
+  </si>
+  <si>
+    <t>hot sprring</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/bioproject/?term=PRJNA362212</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,8 +796,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,6 +843,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -842,7 +914,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -881,6 +953,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -895,6 +968,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1210,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D083C16F-3167-4878-8322-8AAE01B755F8}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I12" zoomScale="132" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" topLeftCell="N18" zoomScale="132" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,6 +1298,8 @@
     <col min="13" max="13" width="13.6328125" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="27.26953125" customWidth="1"/>
+    <col min="17" max="17" width="20.54296875" customWidth="1"/>
+    <col min="18" max="18" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1258,7 +1337,7 @@
         <v>83</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>69</v>
@@ -1306,7 +1385,7 @@
         <v>15</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>73</v>
@@ -1353,8 +1432,8 @@
       <c r="L3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="19" t="s">
-        <v>200</v>
+      <c r="M3" s="20" t="s">
+        <v>198</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>90</v>
@@ -1449,7 +1528,7 @@
         <v>15</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>88</v>
@@ -1498,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N6" s="7" t="s">
         <v>79</v>
@@ -1542,11 +1621,11 @@
       <c r="K7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="16">
+      <c r="L7" s="17">
         <v>-1.5</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N7" s="7" t="s">
         <v>80</v>
@@ -1565,10 +1644,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>47</v>
@@ -1583,10 +1662,10 @@
         <v>49</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>15</v>
@@ -1597,13 +1676,13 @@
       <c r="M8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="N8" s="20" t="s">
-        <v>205</v>
+      <c r="N8" s="21" t="s">
+        <v>203</v>
       </c>
       <c r="O8" s="12"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1642,7 +1721,7 @@
         <v>15</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N9" s="7" t="s">
         <v>96</v>
@@ -1689,10 +1768,10 @@
         <v>15</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="P10" s="6"/>
     </row>
@@ -1720,10 +1799,10 @@
         <v>68</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>15</v>
@@ -1732,13 +1811,13 @@
         <v>15</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N11" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="O11" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>186</v>
       </c>
       <c r="P11" s="13" t="s">
         <v>97</v>
@@ -1748,15 +1827,15 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="P12" s="21"/>
+      <c r="P12" s="22"/>
     </row>
     <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="K13" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
+      <c r="K13" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
     </row>
     <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="K14" s="10" t="s">
@@ -1767,14 +1846,14 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="K15" s="18" t="s">
-        <v>199</v>
-      </c>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="K15" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+    </row>
+    <row r="18" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1818,7 +1897,7 @@
         <v>83</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q18" s="5" t="s">
         <v>69</v>
@@ -1830,7 +1909,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="2"/>
       <c r="B19" s="3">
         <v>1</v>
@@ -1866,7 +1945,7 @@
         <v>112</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>15</v>
@@ -1876,16 +1955,17 @@
       </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="R19" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>199</v>
+      </c>
+      <c r="T19" s="8"/>
+    </row>
+    <row r="20" spans="1:23" ht="28" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="2"/>
       <c r="B20" s="4">
         <v>1</v>
@@ -1915,13 +1995,13 @@
         <v>111</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>112</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>113</v>
+        <v>214</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>15</v>
@@ -1930,42 +2010,56 @@
         <v>15</v>
       </c>
       <c r="P20" s="4"/>
-      <c r="Q20" s="8"/>
+      <c r="Q20" s="8" t="s">
+        <v>208</v>
+      </c>
       <c r="R20" s="8"/>
-      <c r="S20" s="6"/>
-    </row>
-    <row r="21" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S20" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="T20" s="8"/>
+      <c r="U20" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="V20" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="W20" s="6" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="2"/>
       <c r="B21" s="3">
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="K21" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>122</v>
-      </c>
       <c r="L21" s="3" t="s">
         <v>15</v>
       </c>
@@ -1979,90 +2073,100 @@
         <v>15</v>
       </c>
       <c r="P21" s="3"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="6"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="Q21" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="R21" s="12"/>
+      <c r="S21" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="T21" s="8"/>
+    </row>
+    <row r="22" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
       <c r="B22" s="4">
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="J22" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="K22" s="4" t="s">
-        <v>15</v>
+        <v>163</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>112</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>131</v>
+        <v>218</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>15</v>
+        <v>213</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="P22" s="4"/>
-      <c r="Q22" s="8"/>
+      <c r="Q22" s="8" t="s">
+        <v>216</v>
+      </c>
       <c r="R22" s="8"/>
-      <c r="S22" s="6"/>
-    </row>
-    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S22" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="T22" s="8"/>
+    </row>
+    <row r="23" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
       <c r="B23" s="3">
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>140</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>15</v>
@@ -2078,40 +2182,41 @@
       </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
+      <c r="R23" s="24"/>
       <c r="S23" s="6"/>
-    </row>
-    <row r="24" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="T23" s="8"/>
+    </row>
+    <row r="24" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="2"/>
       <c r="B24" s="4">
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="I24" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="K24" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>15</v>
@@ -2127,40 +2232,45 @@
       </c>
       <c r="P24" s="4"/>
       <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
+      <c r="R24" s="24" t="s">
+        <v>219</v>
+      </c>
       <c r="S24" s="6"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="T24" s="14" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="2"/>
       <c r="B25" s="3">
         <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="H25" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="I25" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="H25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="K25" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>15</v>
@@ -2176,41 +2286,42 @@
       </c>
       <c r="P25" s="3"/>
       <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
+      <c r="R25" s="24"/>
       <c r="S25" s="6"/>
-    </row>
-    <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="T25" s="8"/>
+    </row>
+    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="2"/>
       <c r="B26" s="4">
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="H26" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="K26" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="K26" s="4" t="s">
-        <v>165</v>
-      </c>
       <c r="L26" s="4" t="s">
         <v>15</v>
       </c>
@@ -2224,47 +2335,50 @@
         <v>15</v>
       </c>
       <c r="P26" s="4"/>
-      <c r="Q26" s="8"/>
-      <c r="R26" s="8"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="8" t="s">
+        <v>220</v>
+      </c>
       <c r="S26" s="6"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="T26" s="8"/>
+    </row>
+    <row r="27" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="2"/>
       <c r="B27" s="3">
         <v>1</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="F27" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="H27" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="I27" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="K27" s="3" t="s">
-        <v>15</v>
+        <v>225</v>
       </c>
       <c r="L27" s="3" t="s">
         <v>112</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>131</v>
+        <v>222</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>15</v>
@@ -2272,42 +2386,49 @@
       <c r="O27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="8"/>
+      <c r="P27" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q27" s="8" t="s">
+        <v>223</v>
+      </c>
       <c r="R27" s="8"/>
-      <c r="S27" s="6"/>
-    </row>
-    <row r="28" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S27" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="T27" s="8"/>
+    </row>
+    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="2"/>
       <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="G28" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F28" s="4" t="s">
+      <c r="H28" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="I28" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>181</v>
-      </c>
       <c r="K28" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>15</v>
@@ -2323,8 +2444,33 @@
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="8"/>
-      <c r="R28" s="8"/>
+      <c r="R28" s="24"/>
       <c r="S28" s="6"/>
+      <c r="T28" s="8"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="T29" s="8"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="T30" s="8"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="T31" s="8"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="T32" s="8"/>
+    </row>
+    <row r="33" spans="20:20" x14ac:dyDescent="0.35">
+      <c r="T33" s="8"/>
+    </row>
+    <row r="34" spans="20:20" x14ac:dyDescent="0.35">
+      <c r="T34" s="8"/>
+    </row>
+    <row r="35" spans="20:20" x14ac:dyDescent="0.35">
+      <c r="T35" s="8"/>
+    </row>
+    <row r="36" spans="20:20" x14ac:dyDescent="0.35">
+      <c r="T36" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2334,8 +2480,15 @@
     <hyperlink ref="P6" r:id="rId4" display="https://doi.org/10.1099/ijs.0.02366-0" xr:uid="{37D385A3-C90C-41E3-944A-2E8C688449FF}"/>
     <hyperlink ref="P11" r:id="rId5" xr:uid="{20F10F40-4E50-4EE3-9330-D4A21D0FF41D}"/>
     <hyperlink ref="S19" r:id="rId6" display="https://doi.org/10.1007/s10482-013-9959-4" xr:uid="{D4F64722-DBEA-41FE-A08D-E5300B4F990D}"/>
+    <hyperlink ref="V20" r:id="rId7" xr:uid="{F79D97C9-FEDC-4357-A1E6-26BCCD297CC3}"/>
+    <hyperlink ref="W20" r:id="rId8" xr:uid="{33719594-C03D-4C63-A037-D1B2D71FE59D}"/>
+    <hyperlink ref="U20" r:id="rId9" xr:uid="{34932757-8E13-4092-9679-8853553773CA}"/>
+    <hyperlink ref="S20" r:id="rId10" xr:uid="{BF792630-5001-4464-BEE1-0A69697D0F3D}"/>
+    <hyperlink ref="S21" r:id="rId11" xr:uid="{8CA6F93A-C9BC-4483-BAC7-1CB3697683F8}"/>
+    <hyperlink ref="S22" r:id="rId12" xr:uid="{33C98436-9721-4E78-AB58-C88A1D58C5B8}"/>
+    <hyperlink ref="T24" r:id="rId13" xr:uid="{B3F38A68-4986-4F25-8916-BE6CA56E57C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>